<commit_message>
before adding AVL plannings
</commit_message>
<xml_diff>
--- a/IP echipamente statii.xlsx
+++ b/IP echipamente statii.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82FD0EE-3968-4253-A72D-1BE4668A8DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Lista principala"/>
-    <sheet r:id="rId2" sheetId="2" name="panouri"/>
-    <sheet r:id="rId3" sheetId="3" name="user password"/>
-    <sheet r:id="rId4" sheetId="4" name="Inele"/>
+    <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
+    <sheet name="panouri" sheetId="2" r:id="rId2"/>
+    <sheet name="user password" sheetId="3" r:id="rId3"/>
+    <sheet name="Inele" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="315">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -571,9 +577,6 @@
     <t>192.168.95.150</t>
   </si>
   <si>
-    <t>192.168.35.30</t>
-  </si>
-  <si>
     <t>192.168.35.31</t>
   </si>
   <si>
@@ -853,9 +856,6 @@
     <t>Autogara  TVM nemontat</t>
   </si>
   <si>
-    <t>192.168.45.56</t>
-  </si>
-  <si>
     <t>192.168.45.45</t>
   </si>
   <si>
@@ -953,13 +953,27 @@
   </si>
   <si>
     <t>C    55.3</t>
+  </si>
+  <si>
+    <t>Universitate</t>
+  </si>
+  <si>
+    <t>Centrofarm 2</t>
+  </si>
+  <si>
+    <t>x192.168.35.30</t>
+  </si>
+  <si>
+    <t>Carrefour spre centru</t>
+  </si>
+  <si>
+    <t>Carrefour spre BDJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -977,14 +991,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFc55a11"/>
+      <color rgb="FFC55A11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF7c7c7c"/>
+      <color rgb="FF7C7C7C"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1008,7 +1022,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1017,62 +1031,69 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdeebf7"/>
+        <fgColor rgb="FFDEEBF7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b050"/>
+        <fgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b0f0"/>
+        <fgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9dc3e6"/>
+        <fgColor rgb="FF9DC3E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd0cece"/>
+        <fgColor rgb="FFD0CECE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70ad47"/>
+        <fgColor rgb="FF70AD47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92d050"/>
+        <fgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffd966"/>
+        <fgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFff0000"/>
+        <fgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffc000"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1086,16 +1107,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1104,19 +1125,19 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -1125,7 +1146,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1140,7 +1161,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1155,7 +1176,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1164,13 +1185,13 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1185,7 +1206,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1200,7 +1221,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1275,7 +1296,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1284,13 +1305,13 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1309,16 +1330,16 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -1362,217 +1383,214 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="68">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1583,10 +1601,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1624,71 +1642,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1716,7 +1734,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1739,11 +1757,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1752,13 +1770,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1768,7 +1786,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1777,7 +1795,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1786,7 +1804,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1794,10 +1812,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1862,32 +1880,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="25" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="67" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="44.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="2.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="65" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>171</v>
       </c>
@@ -1918,7 +1937,7 @@
       <c r="L1" s="33"/>
       <c r="M1" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1947,7 +1966,7 @@
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25">
+    <row r="3" spans="1:13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1976,7 +1995,7 @@
       <c r="L3" s="33"/>
       <c r="M3" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -1990,55 +2009,55 @@
       <c r="E4" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="67" t="s">
+        <v>312</v>
+      </c>
+      <c r="G4" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="H4" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="I4" s="31" t="s">
         <v>186</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>187</v>
       </c>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>63</v>
+        <v>313</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="34" t="s">
         <v>190</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>191</v>
       </c>
       <c r="H5" s="30"/>
       <c r="I5" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="33"/>
       <c r="M5" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -2049,11 +2068,11 @@
         <v>66</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="30"/>
@@ -2063,7 +2082,7 @@
       <c r="L6" s="33"/>
       <c r="M6" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -2082,12 +2101,12 @@
       <c r="L7" s="33"/>
       <c r="M7" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>69</v>
@@ -2095,7 +2114,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="35"/>
       <c r="F8" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="30"/>
@@ -2105,7 +2124,7 @@
       <c r="L8" s="31"/>
       <c r="M8" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -2118,10 +2137,10 @@
       <c r="D9" s="20"/>
       <c r="E9" s="35"/>
       <c r="F9" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>197</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>198</v>
       </c>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
@@ -2130,25 +2149,25 @@
       <c r="L9" s="31"/>
       <c r="M9" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>95</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>201</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>202</v>
       </c>
       <c r="H10" s="30"/>
       <c r="I10" s="30"/>
@@ -2157,7 +2176,7 @@
       <c r="L10" s="31"/>
       <c r="M10" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -2168,11 +2187,11 @@
         <v>77</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="11"/>
@@ -2182,7 +2201,7 @@
       <c r="L11" s="31"/>
       <c r="M11" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -2195,7 +2214,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="35"/>
       <c r="F12" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="11"/>
@@ -2205,7 +2224,7 @@
       <c r="L12" s="31"/>
       <c r="M12" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="32.25">
+    <row r="13" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>12</v>
       </c>
@@ -2217,24 +2236,24 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="34" t="s">
         <v>207</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>208</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
       <c r="M13" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -2245,13 +2264,13 @@
         <v>83</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>211</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>212</v>
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="11"/>
@@ -2261,7 +2280,7 @@
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -2272,16 +2291,16 @@
         <v>86</v>
       </c>
       <c r="D15" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="F15" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="G15" s="41" t="s">
         <v>215</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>216</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -2290,7 +2309,7 @@
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="30.75">
+    <row r="16" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>15</v>
       </c>
@@ -2303,10 +2322,10 @@
       <c r="D16" s="20"/>
       <c r="E16" s="35"/>
       <c r="F16" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" s="42" t="s">
         <v>217</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>218</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -2315,7 +2334,7 @@
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="13.9">
+    <row r="17" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>16</v>
       </c>
@@ -2326,17 +2345,17 @@
         <v>91</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="H17" s="30" t="s">
         <v>221</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>222</v>
       </c>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
@@ -2344,7 +2363,7 @@
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>17</v>
       </c>
@@ -2355,11 +2374,11 @@
         <v>94</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G18" s="34"/>
       <c r="H18" s="30"/>
@@ -2369,12 +2388,12 @@
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>74</v>
@@ -2383,10 +2402,10 @@
       <c r="E19" s="35"/>
       <c r="F19" s="17"/>
       <c r="G19" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="H19" s="30" t="s">
         <v>226</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>227</v>
       </c>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
@@ -2394,7 +2413,7 @@
       <c r="L19" s="33"/>
       <c r="M19" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="15">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
@@ -2405,11 +2424,11 @@
         <v>98</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="30"/>
@@ -2419,7 +2438,7 @@
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>20</v>
       </c>
@@ -2432,7 +2451,7 @@
       <c r="D21" s="20"/>
       <c r="E21" s="35"/>
       <c r="F21" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="30"/>
@@ -2442,7 +2461,7 @@
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>21</v>
       </c>
@@ -2461,7 +2480,7 @@
       <c r="L22" s="33"/>
       <c r="M22" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="33">
+    <row r="23" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>22</v>
       </c>
@@ -2472,14 +2491,14 @@
         <v>104</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E23" s="35"/>
       <c r="F23" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="G23" s="34" t="s">
         <v>232</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>233</v>
       </c>
       <c r="H23" s="30"/>
       <c r="I23" s="31"/>
@@ -2488,12 +2507,12 @@
       <c r="L23" s="33"/>
       <c r="M23" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>63</v>
+        <v>314</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>106</v>
@@ -2501,10 +2520,10 @@
       <c r="D24" s="43"/>
       <c r="E24" s="35"/>
       <c r="F24" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="34" t="s">
         <v>234</v>
-      </c>
-      <c r="G24" s="34" t="s">
-        <v>235</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="31"/>
@@ -2513,7 +2532,7 @@
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>24</v>
       </c>
@@ -2525,13 +2544,13 @@
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="G25" s="36" t="s">
         <v>237</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>238</v>
       </c>
       <c r="H25" s="30"/>
       <c r="I25" s="31"/>
@@ -2540,7 +2559,7 @@
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>25</v>
       </c>
@@ -2551,11 +2570,11 @@
         <v>110</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G26" s="34"/>
       <c r="H26" s="30"/>
@@ -2565,7 +2584,7 @@
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>26</v>
       </c>
@@ -2584,7 +2603,7 @@
       <c r="L27" s="33"/>
       <c r="M27" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>27</v>
       </c>
@@ -2603,7 +2622,7 @@
       <c r="L28" s="33"/>
       <c r="M28" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="31.899999999999995">
+    <row r="29" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>28</v>
       </c>
@@ -2614,14 +2633,14 @@
         <v>114</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="G29" s="36" t="s">
         <v>242</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>243</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="31"/>
@@ -2630,7 +2649,7 @@
       <c r="L29" s="33"/>
       <c r="M29" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>29</v>
       </c>
@@ -2643,7 +2662,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="35"/>
       <c r="F30" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="30"/>
@@ -2653,7 +2672,7 @@
       <c r="L30" s="33"/>
       <c r="M30" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>30</v>
       </c>
@@ -2666,10 +2685,10 @@
       <c r="D31" s="20"/>
       <c r="E31" s="35"/>
       <c r="F31" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="G31" s="34" t="s">
         <v>245</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>246</v>
       </c>
       <c r="H31" s="30"/>
       <c r="I31" s="31"/>
@@ -2678,7 +2697,7 @@
       <c r="L31" s="33"/>
       <c r="M31" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>31</v>
       </c>
@@ -2697,7 +2716,7 @@
       <c r="L32" s="33"/>
       <c r="M32" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>32</v>
       </c>
@@ -2708,11 +2727,11 @@
         <v>121</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E33" s="35"/>
       <c r="F33" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G33" s="34"/>
       <c r="H33" s="30"/>
@@ -2722,7 +2741,7 @@
       <c r="L33" s="33"/>
       <c r="M33" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="31.899999999999995">
+    <row r="34" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>33</v>
       </c>
@@ -2733,14 +2752,14 @@
         <v>124</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="G34" s="36" t="s">
         <v>250</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>251</v>
       </c>
       <c r="H34" s="40"/>
       <c r="I34" s="31"/>
@@ -2749,7 +2768,7 @@
       <c r="L34" s="33"/>
       <c r="M34" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>34</v>
       </c>
@@ -2762,13 +2781,13 @@
       <c r="D35" s="20"/>
       <c r="E35" s="35"/>
       <c r="F35" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="G35" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="G35" s="42" t="s">
+      <c r="H35" s="40" t="s">
         <v>253</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>254</v>
       </c>
       <c r="I35" s="31"/>
       <c r="J35" s="31"/>
@@ -2776,12 +2795,12 @@
       <c r="L35" s="33"/>
       <c r="M35" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>35</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>128</v>
@@ -2789,13 +2808,13 @@
       <c r="D36" s="17"/>
       <c r="E36" s="35"/>
       <c r="F36" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="G36" s="34" t="s">
+      <c r="H36" s="30" t="s">
         <v>257</v>
-      </c>
-      <c r="H36" s="30" t="s">
-        <v>258</v>
       </c>
       <c r="I36" s="31"/>
       <c r="J36" s="31"/>
@@ -2803,7 +2822,7 @@
       <c r="L36" s="33"/>
       <c r="M36" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>36</v>
       </c>
@@ -2816,7 +2835,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="35"/>
       <c r="F37" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G37" s="34"/>
       <c r="H37" s="30"/>
@@ -2826,7 +2845,7 @@
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>37</v>
       </c>
@@ -2837,14 +2856,14 @@
         <v>133</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E38" s="35"/>
       <c r="F38" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="G38" s="34" t="s">
         <v>261</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>262</v>
       </c>
       <c r="H38" s="30"/>
       <c r="I38" s="31"/>
@@ -2853,7 +2872,7 @@
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>38</v>
       </c>
@@ -2866,7 +2885,7 @@
       <c r="D39" s="20"/>
       <c r="E39" s="35"/>
       <c r="F39" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G39" s="34"/>
       <c r="H39" s="30"/>
@@ -2876,7 +2895,7 @@
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>39</v>
       </c>
@@ -2895,7 +2914,7 @@
       <c r="L40" s="33"/>
       <c r="M40" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>40</v>
       </c>
@@ -2908,10 +2927,10 @@
       <c r="D41" s="22"/>
       <c r="E41" s="38"/>
       <c r="F41" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="G41" s="39" t="s">
         <v>264</v>
-      </c>
-      <c r="G41" s="39" t="s">
-        <v>265</v>
       </c>
       <c r="H41" s="30"/>
       <c r="I41" s="31"/>
@@ -2920,7 +2939,7 @@
       <c r="L41" s="33"/>
       <c r="M41" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>41</v>
       </c>
@@ -2939,7 +2958,7 @@
       <c r="L42" s="33"/>
       <c r="M42" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>42</v>
       </c>
@@ -2958,7 +2977,7 @@
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="33">
+    <row r="44" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>43</v>
       </c>
@@ -2969,10 +2988,10 @@
       <c r="D44" s="20"/>
       <c r="E44" s="35"/>
       <c r="F44" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="G44" s="34" t="s">
         <v>266</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>267</v>
       </c>
       <c r="H44" s="30"/>
       <c r="I44" s="31"/>
@@ -2981,7 +3000,7 @@
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>44</v>
       </c>
@@ -2992,10 +3011,10 @@
       <c r="D45" s="20"/>
       <c r="E45" s="35"/>
       <c r="F45" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="G45" s="34" t="s">
         <v>268</v>
-      </c>
-      <c r="G45" s="34" t="s">
-        <v>269</v>
       </c>
       <c r="H45" s="30"/>
       <c r="I45" s="31"/>
@@ -3004,7 +3023,7 @@
       <c r="L45" s="33"/>
       <c r="M45" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>45</v>
       </c>
@@ -3016,10 +3035,10 @@
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="F46" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>271</v>
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="30"/>
@@ -3029,7 +3048,7 @@
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>46</v>
       </c>
@@ -3043,10 +3062,10 @@
       <c r="E47" s="35"/>
       <c r="F47" s="36"/>
       <c r="G47" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="H47" s="40" t="s">
         <v>272</v>
-      </c>
-      <c r="H47" s="40" t="s">
-        <v>273</v>
       </c>
       <c r="I47" s="31"/>
       <c r="J47" s="31"/>
@@ -3054,7 +3073,7 @@
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>47</v>
       </c>
@@ -3065,14 +3084,14 @@
         <v>151</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E48" s="35"/>
       <c r="F48" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G48" s="34" t="s">
         <v>275</v>
-      </c>
-      <c r="G48" s="34" t="s">
-        <v>276</v>
       </c>
       <c r="H48" s="30"/>
       <c r="I48" s="31"/>
@@ -3081,34 +3100,32 @@
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>48</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D49" s="45" t="s">
-        <v>278</v>
-      </c>
+      <c r="D49" s="66"/>
       <c r="E49" s="35"/>
       <c r="F49" s="17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H49" s="30"/>
       <c r="I49" s="31"/>
       <c r="J49" s="31"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="47"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="46"/>
       <c r="M49" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>49</v>
       </c>
@@ -3119,13 +3136,13 @@
         <v>155</v>
       </c>
       <c r="D50" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="F50" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="E50" s="35" t="s">
-        <v>282</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>283</v>
       </c>
       <c r="G50" s="34"/>
       <c r="H50" s="30"/>
@@ -3135,23 +3152,23 @@
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>50</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="48" t="s">
-        <v>284</v>
+      <c r="C51" s="47" t="s">
+        <v>282</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="35"/>
       <c r="F51" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="G51" s="49" t="s">
-        <v>286</v>
+        <v>283</v>
+      </c>
+      <c r="G51" s="48" t="s">
+        <v>284</v>
       </c>
       <c r="H51" s="30"/>
       <c r="I51" s="31"/>
@@ -3160,7 +3177,7 @@
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>51</v>
       </c>
@@ -3173,23 +3190,23 @@
       <c r="D52" s="20"/>
       <c r="E52" s="35"/>
       <c r="F52" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="G52" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="H52" s="49" t="s">
         <v>287</v>
       </c>
-      <c r="G52" s="49" t="s">
+      <c r="I52" s="50" t="s">
         <v>288</v>
-      </c>
-      <c r="H52" s="50" t="s">
-        <v>289</v>
-      </c>
-      <c r="I52" s="51" t="s">
-        <v>290</v>
       </c>
       <c r="J52" s="31"/>
       <c r="K52" s="31"/>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="33.6">
+    <row r="53" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>52</v>
       </c>
@@ -3202,10 +3219,10 @@
       <c r="D53" s="20"/>
       <c r="E53" s="35"/>
       <c r="F53" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H53" s="30"/>
       <c r="I53" s="31"/>
@@ -3214,19 +3231,19 @@
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="30.600000000000005">
+    <row r="54" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>53</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="52" t="s">
-        <v>293</v>
-      </c>
-      <c r="D54" s="52"/>
-      <c r="E54" s="53" t="s">
-        <v>294</v>
+      <c r="C54" s="51" t="s">
+        <v>291</v>
+      </c>
+      <c r="D54" s="51"/>
+      <c r="E54" s="52" t="s">
+        <v>292</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="34"/>
@@ -3237,17 +3254,19 @@
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="30.600000000000005">
-      <c r="A55" s="54"/>
+    <row r="55" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="53">
+        <v>54</v>
+      </c>
       <c r="B55" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="D55" s="51"/>
+      <c r="E55" s="52" t="s">
         <v>295</v>
-      </c>
-      <c r="C55" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="D55" s="52"/>
-      <c r="E55" s="53" t="s">
-        <v>297</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="34"/>
@@ -3258,9 +3277,9 @@
       <c r="L55" s="33"/>
       <c r="M55" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="36">
+    <row r="56" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>163</v>
@@ -3270,10 +3289,10 @@
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="35" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G56" s="34"/>
       <c r="H56" s="30"/>
@@ -3283,47 +3302,51 @@
       <c r="L56" s="33"/>
       <c r="M56" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="40.15">
-      <c r="A57" s="55"/>
-      <c r="B57" s="20" t="s">
-        <v>165</v>
+    <row r="57" spans="1:13" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="23">
+        <v>56</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>310</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>166</v>
       </c>
       <c r="D57" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="E57" s="51"/>
+      <c r="F57" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="G57" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="E57" s="52"/>
-      <c r="F57" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="G57" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="H57" s="56"/>
+      <c r="H57" s="54"/>
       <c r="I57" s="31"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="55"/>
-      <c r="B58" s="20" t="s">
-        <v>168</v>
+    <row r="58" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="23">
+        <v>57</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>311</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>169</v>
       </c>
       <c r="D58" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="F58" s="17" t="s">
         <v>303</v>
-      </c>
-      <c r="E58" s="35" t="s">
-        <v>304</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>305</v>
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="30"/>
@@ -3333,22 +3356,22 @@
       <c r="L58" s="11"/>
       <c r="M58" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="15"/>
-      <c r="C59" s="57" t="s">
+      <c r="C59" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="D59" s="57" t="s">
+      <c r="D59" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="E59" s="58" t="s">
+      <c r="E59" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="F59" s="59" t="s">
+      <c r="F59" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G59" s="58" t="s">
+      <c r="G59" s="56" t="s">
         <v>47</v>
       </c>
       <c r="H59" s="15"/>
@@ -3358,14 +3381,14 @@
       <c r="L59" s="11"/>
       <c r="M59" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="33"/>
       <c r="C60" s="30"/>
-      <c r="D60" s="60"/>
+      <c r="D60" s="58"/>
       <c r="E60" s="33"/>
-      <c r="F60" s="61" t="s">
-        <v>306</v>
+      <c r="F60" s="59" t="s">
+        <v>304</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
@@ -3375,14 +3398,14 @@
       <c r="L60" s="11"/>
       <c r="M60" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="61" t="s">
-        <v>307</v>
+      <c r="F61" s="59" t="s">
+        <v>305</v>
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
@@ -3392,50 +3415,50 @@
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
-      <c r="B62" s="62"/>
+      <c r="B62" s="60"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="64" t="s">
-        <v>308</v>
-      </c>
-      <c r="G62" s="65"/>
-      <c r="H62" s="66"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="62" t="s">
+        <v>306</v>
+      </c>
+      <c r="G62" s="63"/>
+      <c r="H62" s="64"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
       <c r="L62" s="11"/>
       <c r="M62" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="B63" s="62"/>
+        <v>307</v>
+      </c>
+      <c r="B63" s="60"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
-      <c r="E63" s="63"/>
-      <c r="F63" s="64" t="s">
-        <v>310</v>
-      </c>
-      <c r="G63" s="65"/>
-      <c r="H63" s="66"/>
+      <c r="E63" s="61"/>
+      <c r="F63" s="62" t="s">
+        <v>308</v>
+      </c>
+      <c r="G63" s="63"/>
+      <c r="H63" s="64"/>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
       <c r="K63" s="11"/>
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="61" t="s">
-        <v>311</v>
+      <c r="F64" s="59" t="s">
+        <v>309</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="15"/>
@@ -3451,7 +3474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3461,15 +3484,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="25" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="35.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16">
         <v>1</v>
       </c>
@@ -3487,7 +3509,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>2</v>
       </c>
@@ -3505,7 +3527,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>3</v>
       </c>
@@ -3523,7 +3545,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>4</v>
       </c>
@@ -3541,7 +3563,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>5</v>
       </c>
@@ -3559,7 +3581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>6</v>
       </c>
@@ -3571,7 +3593,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>7</v>
       </c>
@@ -3591,7 +3613,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>8</v>
       </c>
@@ -3609,7 +3631,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>9</v>
       </c>
@@ -3627,7 +3649,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>10</v>
       </c>
@@ -3643,7 +3665,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>11</v>
       </c>
@@ -3659,7 +3681,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>12</v>
       </c>
@@ -3675,7 +3697,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>13</v>
       </c>
@@ -3693,7 +3715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>14</v>
       </c>
@@ -3709,7 +3731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>15</v>
       </c>
@@ -3727,7 +3749,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>16</v>
       </c>
@@ -3745,7 +3767,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>17</v>
       </c>
@@ -3761,7 +3783,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>18</v>
       </c>
@@ -3779,7 +3801,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>19</v>
       </c>
@@ -3799,7 +3821,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>20</v>
       </c>
@@ -3819,7 +3841,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>21</v>
       </c>
@@ -3831,7 +3853,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>22</v>
       </c>
@@ -3851,7 +3873,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>23</v>
       </c>
@@ -3871,7 +3893,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>24</v>
       </c>
@@ -3889,7 +3911,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>25</v>
       </c>
@@ -3905,7 +3927,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>26</v>
       </c>
@@ -3917,7 +3939,7 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>27</v>
       </c>
@@ -3929,7 +3951,7 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>28</v>
       </c>
@@ -3945,7 +3967,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>29</v>
       </c>
@@ -3961,7 +3983,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>30</v>
       </c>
@@ -3977,7 +3999,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>31</v>
       </c>
@@ -3989,7 +4011,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>32</v>
       </c>
@@ -4007,7 +4029,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>33</v>
       </c>
@@ -4025,7 +4047,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>34</v>
       </c>
@@ -4041,7 +4063,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>35</v>
       </c>
@@ -4059,7 +4081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>36</v>
       </c>
@@ -4077,7 +4099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>37</v>
       </c>
@@ -4093,7 +4115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>38</v>
       </c>
@@ -4109,7 +4131,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>39</v>
       </c>
@@ -4123,7 +4145,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>136</v>
       </c>
@@ -4139,7 +4161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>41</v>
       </c>
@@ -4151,7 +4173,7 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>42</v>
       </c>
@@ -4163,7 +4185,7 @@
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>43</v>
       </c>
@@ -4177,7 +4199,7 @@
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>44</v>
       </c>
@@ -4195,7 +4217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>1</v>
       </c>
@@ -4211,7 +4233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>46</v>
       </c>
@@ -4227,7 +4249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>47</v>
       </c>
@@ -4243,7 +4265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>115</v>
       </c>
@@ -4259,7 +4281,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>75</v>
       </c>
@@ -4275,7 +4297,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>50</v>
       </c>
@@ -4291,7 +4313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>81</v>
       </c>
@@ -4307,7 +4329,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>74</v>
       </c>
@@ -4323,7 +4345,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
       <c r="B53" s="21" t="s">
         <v>162</v>
@@ -4333,7 +4355,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23">
         <v>68</v>
       </c>
@@ -4349,7 +4371,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="20" t="s">
         <v>165</v>
@@ -4365,7 +4387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
         <v>66</v>
       </c>
@@ -4381,7 +4403,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15" t="s">
@@ -4397,7 +4419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4407,12 +4429,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -4423,7 +4445,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
@@ -4434,7 +4456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>50</v>
       </c>
@@ -4445,7 +4467,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
@@ -4456,102 +4478,102 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -4562,7 +4584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4572,14 +4594,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="44.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="40.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="27.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4590,7 +4612,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4607,7 +4629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
@@ -4624,7 +4646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -4639,7 +4661,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="42.75">
+    <row r="5" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
@@ -4652,7 +4674,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="29.25">
+    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>17</v>
@@ -4663,7 +4685,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>19</v>
@@ -4674,7 +4696,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>21</v>
@@ -4685,7 +4707,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>23</v>
@@ -4696,7 +4718,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
@@ -4705,7 +4727,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
@@ -4714,7 +4736,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
@@ -4723,7 +4745,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11" t="s">
@@ -4732,7 +4754,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
@@ -4741,7 +4763,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
@@ -4750,7 +4772,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11" t="s">
@@ -4759,7 +4781,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
@@ -4768,7 +4790,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
@@ -4777,7 +4799,7 @@
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
@@ -4786,7 +4808,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
@@ -4795,7 +4817,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11" t="s">
@@ -4804,7 +4826,7 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
@@ -4813,7 +4835,7 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
@@ -4822,7 +4844,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
@@ -4831,7 +4853,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11" t="s">
@@ -4840,7 +4862,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
@@ -4849,7 +4871,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
@@ -4858,7 +4880,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11" t="s">
@@ -4867,7 +4889,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11" t="s">
@@ -4876,7 +4898,7 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11" t="s">
@@ -4885,7 +4907,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11" t="s">

</xml_diff>

<commit_message>
added network.py and processes.py
</commit_message>
<xml_diff>
--- a/IP echipamente statii.xlsx
+++ b/IP echipamente statii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82FD0EE-3968-4253-A72D-1BE4668A8DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F829CE-63D5-4C6D-9458-BBFB8F664350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="316">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -961,13 +961,16 @@
     <t>Centrofarm 2</t>
   </si>
   <si>
+    <t>Carrefour spre centru</t>
+  </si>
+  <si>
+    <t>Carrefour spre BDJ</t>
+  </si>
+  <si>
+    <t>Sticla</t>
+  </si>
+  <si>
     <t>x192.168.35.30</t>
-  </si>
-  <si>
-    <t>Carrefour spre centru</t>
-  </si>
-  <si>
-    <t>Carrefour spre BDJ</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1578,6 +1581,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1886,8 +1901,8 @@
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,7 +2025,7 @@
         <v>183</v>
       </c>
       <c r="F4" s="67" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>184</v>
@@ -2031,7 +2046,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>64</v>
@@ -2512,7 +2527,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>106</v>
@@ -2921,15 +2936,15 @@
       <c r="B41" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="19" t="s">
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="68" t="s">
         <v>263</v>
       </c>
-      <c r="G41" s="39" t="s">
+      <c r="G41" s="71" t="s">
         <v>264</v>
       </c>
       <c r="H41" s="30"/>
@@ -2981,8 +2996,8 @@
       <c r="A44" s="16">
         <v>43</v>
       </c>
-      <c r="B44" s="20" t="s">
-        <v>141</v>
+      <c r="B44" s="17" t="s">
+        <v>314</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="20"/>

</xml_diff>

<commit_message>
changing in whatsapp module - putting messages in queue in read from it on event(when a meesage has comed in)
</commit_message>
<xml_diff>
--- a/IP echipamente statii.xlsx
+++ b/IP echipamente statii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F829CE-63D5-4C6D-9458-BBFB8F664350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83A5EF4-F90D-4DC4-8D62-83BC46ABDEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="333">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -607,9 +607,6 @@
     <t>192.168.25.26</t>
   </si>
   <si>
-    <t>Grup scolar 2 spre primarie</t>
-  </si>
-  <si>
     <t>192.168.25.28</t>
   </si>
   <si>
@@ -787,18 +784,12 @@
     <t>55 adaugat fata de lista originala 8.10.2021</t>
   </si>
   <si>
-    <t>Curcubeu spre policlinica</t>
-  </si>
-  <si>
     <t>192.168.55.42</t>
   </si>
   <si>
     <t>192.168.55.48 statie ap 192.168.55.49 cctv</t>
   </si>
   <si>
-    <t>pe 49 eth disabled</t>
-  </si>
-  <si>
     <t>192.168.55.32</t>
   </si>
   <si>
@@ -853,9 +844,6 @@
     <t>192.168.45.57 (CCTV) 192.168.45.60 statie</t>
   </si>
   <si>
-    <t>Autogara  TVM nemontat</t>
-  </si>
-  <si>
     <t>192.168.45.45</t>
   </si>
   <si>
@@ -871,9 +859,6 @@
     <t>192.168.35.62</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>192.168.35.64</t>
   </si>
   <si>
@@ -971,6 +956,72 @@
   </si>
   <si>
     <t>x192.168.35.30</t>
+  </si>
+  <si>
+    <t>192.168.45.240</t>
+  </si>
+  <si>
+    <t>Obcini Flori</t>
+  </si>
+  <si>
+    <t>Orizont spre Centru</t>
+  </si>
+  <si>
+    <t>Orizont spre BDJ</t>
+  </si>
+  <si>
+    <t>Curcubeu spre catedrala</t>
+  </si>
+  <si>
+    <t>Policlinca spre BDJ</t>
+  </si>
+  <si>
+    <t>Grup scolar spre BDJ</t>
+  </si>
+  <si>
+    <t>Centru spre primarie</t>
+  </si>
+  <si>
+    <t>Grup scolar spre centru</t>
+  </si>
+  <si>
+    <t>Mobila spre curcubeu</t>
+  </si>
+  <si>
+    <t>Bazar 2 Lidl</t>
+  </si>
+  <si>
+    <t>Bazar 1</t>
+  </si>
+  <si>
+    <t>Mobila spre obcini</t>
+  </si>
+  <si>
+    <t>Catedrala spre policlinica</t>
+  </si>
+  <si>
+    <t>Autogara TVM nemontat</t>
+  </si>
+  <si>
+    <t>192.168.35.58</t>
+  </si>
+  <si>
+    <t>Curcubeu spre obcini</t>
+  </si>
+  <si>
+    <t>x192.168.45.48</t>
+  </si>
+  <si>
+    <t>pe 49 eth disabled ,pe fibra de la statia de vizavi</t>
+  </si>
+  <si>
+    <t>x192.168.25.37</t>
+  </si>
+  <si>
+    <t>x192.168.35.63</t>
+  </si>
+  <si>
+    <t>x192.168.25.45</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1076,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1096,6 +1147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1385,7 +1442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1519,9 +1576,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1534,9 +1588,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1585,14 +1636,29 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1901,18 +1967,18 @@
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="12" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="65" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="63" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
@@ -1986,7 +2052,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>59</v>
+        <v>313</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>60</v>
@@ -2024,8 +2090,8 @@
       <c r="E4" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F4" s="67" t="s">
-        <v>315</v>
+      <c r="F4" s="65" t="s">
+        <v>310</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>184</v>
@@ -2046,7 +2112,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>64</v>
@@ -2077,7 +2143,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>65</v>
+        <v>322</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>66</v>
@@ -2121,7 +2187,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>194</v>
+        <v>319</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>69</v>
@@ -2129,7 +2195,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="35"/>
       <c r="F8" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="30"/>
@@ -2144,7 +2210,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>71</v>
+        <v>318</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>72</v>
@@ -2152,10 +2218,10 @@
       <c r="D9" s="20"/>
       <c r="E9" s="35"/>
       <c r="F9" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>196</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>197</v>
       </c>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
@@ -2169,20 +2235,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>95</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>200</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>201</v>
       </c>
       <c r="H10" s="30"/>
       <c r="I10" s="30"/>
@@ -2202,11 +2268,11 @@
         <v>77</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="11"/>
@@ -2229,7 +2295,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="35"/>
       <c r="F12" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="11"/>
@@ -2244,24 +2310,24 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>80</v>
+        <v>312</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>81</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="34" t="s">
         <v>206</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>207</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
@@ -2273,19 +2339,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>82</v>
+        <v>320</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>83</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>210</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>211</v>
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="11"/>
@@ -2300,22 +2366,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>85</v>
+        <v>315</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D15" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="F15" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="G15" s="41" t="s">
         <v>214</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>215</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -2337,10 +2403,10 @@
       <c r="D16" s="20"/>
       <c r="E16" s="35"/>
       <c r="F16" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G16" s="42" t="s">
         <v>216</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>217</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -2354,23 +2420,23 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>90</v>
+        <v>324</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>91</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G17" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="H17" s="30" t="s">
         <v>220</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>221</v>
       </c>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
@@ -2383,17 +2449,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>93</v>
+        <v>316</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>94</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G18" s="34"/>
       <c r="H18" s="30"/>
@@ -2408,19 +2474,21 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="65" t="s">
+        <v>332</v>
+      </c>
       <c r="G19" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="H19" s="30" t="s">
         <v>225</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>226</v>
       </c>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
@@ -2439,11 +2507,11 @@
         <v>98</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="30"/>
@@ -2458,7 +2526,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>68</v>
+        <v>317</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>101</v>
@@ -2466,7 +2534,7 @@
       <c r="D21" s="20"/>
       <c r="E21" s="35"/>
       <c r="F21" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="30"/>
@@ -2500,20 +2568,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>103</v>
+        <v>321</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>104</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E23" s="35"/>
       <c r="F23" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G23" s="34" t="s">
         <v>231</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>232</v>
       </c>
       <c r="H23" s="30"/>
       <c r="I23" s="31"/>
@@ -2527,7 +2595,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>106</v>
@@ -2535,10 +2603,10 @@
       <c r="D24" s="43"/>
       <c r="E24" s="35"/>
       <c r="F24" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="G24" s="34" t="s">
         <v>233</v>
-      </c>
-      <c r="G24" s="34" t="s">
-        <v>234</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="31"/>
@@ -2552,20 +2620,20 @@
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>59</v>
+        <v>314</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>108</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="G25" s="36" t="s">
         <v>236</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>237</v>
       </c>
       <c r="H25" s="30"/>
       <c r="I25" s="31"/>
@@ -2585,11 +2653,11 @@
         <v>110</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G26" s="34"/>
       <c r="H26" s="30"/>
@@ -2603,14 +2671,14 @@
       <c r="A27" s="16">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="34"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="72"/>
       <c r="H27" s="30"/>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -2622,14 +2690,14 @@
       <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="34"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="72"/>
       <c r="H28" s="30"/>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -2648,14 +2716,14 @@
         <v>114</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" s="36" t="s">
         <v>241</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>242</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="31"/>
@@ -2677,7 +2745,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="35"/>
       <c r="F30" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="30"/>
@@ -2700,10 +2768,10 @@
       <c r="D31" s="20"/>
       <c r="E31" s="35"/>
       <c r="F31" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="G31" s="34" t="s">
         <v>244</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>245</v>
       </c>
       <c r="H31" s="30"/>
       <c r="I31" s="31"/>
@@ -2742,11 +2810,11 @@
         <v>121</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E33" s="35"/>
       <c r="F33" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G33" s="34"/>
       <c r="H33" s="30"/>
@@ -2767,14 +2835,14 @@
         <v>124</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="G34" s="36" t="s">
         <v>249</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>250</v>
       </c>
       <c r="H34" s="40"/>
       <c r="I34" s="31"/>
@@ -2796,13 +2864,13 @@
       <c r="D35" s="20"/>
       <c r="E35" s="35"/>
       <c r="F35" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="G35" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="G35" s="42" t="s">
+      <c r="H35" s="40" t="s">
         <v>252</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>253</v>
       </c>
       <c r="I35" s="31"/>
       <c r="J35" s="31"/>
@@ -2814,8 +2882,8 @@
       <c r="A36" s="16">
         <v>35</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>254</v>
+      <c r="B36" s="17" t="s">
+        <v>327</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>128</v>
@@ -2823,13 +2891,13 @@
       <c r="D36" s="17"/>
       <c r="E36" s="35"/>
       <c r="F36" s="17" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>257</v>
+        <v>329</v>
       </c>
       <c r="I36" s="31"/>
       <c r="J36" s="31"/>
@@ -2841,8 +2909,8 @@
       <c r="A37" s="16">
         <v>36</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>82</v>
+      <c r="B37" s="17" t="s">
+        <v>323</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>130</v>
@@ -2850,7 +2918,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="35"/>
       <c r="F37" s="17" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G37" s="34"/>
       <c r="H37" s="30"/>
@@ -2871,14 +2939,14 @@
         <v>133</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E38" s="35"/>
       <c r="F38" s="17" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H38" s="30"/>
       <c r="I38" s="31"/>
@@ -2900,7 +2968,7 @@
       <c r="D39" s="20"/>
       <c r="E39" s="35"/>
       <c r="F39" s="17" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G39" s="34"/>
       <c r="H39" s="30"/>
@@ -2936,16 +3004,18 @@
       <c r="B41" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="69"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="68" t="s">
-        <v>263</v>
-      </c>
-      <c r="G41" s="71" t="s">
-        <v>264</v>
+      <c r="D41" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="E41" s="67"/>
+      <c r="F41" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="G41" s="68" t="s">
+        <v>261</v>
       </c>
       <c r="H41" s="30"/>
       <c r="I41" s="31"/>
@@ -2997,16 +3067,18 @@
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C44" s="17"/>
+        <v>309</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>328</v>
+      </c>
       <c r="D44" s="20"/>
       <c r="E44" s="35"/>
       <c r="F44" s="17" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H44" s="30"/>
       <c r="I44" s="31"/>
@@ -3022,14 +3094,16 @@
       <c r="B45" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="65" t="s">
+        <v>330</v>
+      </c>
       <c r="D45" s="20"/>
       <c r="E45" s="35"/>
       <c r="F45" s="17" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H45" s="30"/>
       <c r="I45" s="31"/>
@@ -3050,10 +3124,10 @@
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="35" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="30"/>
@@ -3075,12 +3149,14 @@
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="35"/>
-      <c r="F47" s="36"/>
+      <c r="F47" s="36" t="s">
+        <v>326</v>
+      </c>
       <c r="G47" s="34" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H47" s="40" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I47" s="31"/>
       <c r="J47" s="31"/>
@@ -3099,14 +3175,14 @@
         <v>151</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E48" s="35"/>
       <c r="F48" s="17" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G48" s="34" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H48" s="30"/>
       <c r="I48" s="31"/>
@@ -3119,19 +3195,19 @@
       <c r="A49" s="16">
         <v>48</v>
       </c>
-      <c r="B49" s="20" t="s">
-        <v>276</v>
+      <c r="B49" s="17" t="s">
+        <v>325</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D49" s="66"/>
+      <c r="D49" s="64"/>
       <c r="E49" s="35"/>
       <c r="F49" s="17" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H49" s="30"/>
       <c r="I49" s="31"/>
@@ -3151,13 +3227,13 @@
         <v>155</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G50" s="34"/>
       <c r="H50" s="30"/>
@@ -3174,16 +3250,16 @@
       <c r="B51" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="47" t="s">
-        <v>282</v>
+      <c r="C51" s="74" t="s">
+        <v>331</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="35"/>
       <c r="F51" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="G51" s="48" t="s">
-        <v>284</v>
+        <v>278</v>
+      </c>
+      <c r="G51" s="47" t="s">
+        <v>279</v>
       </c>
       <c r="H51" s="30"/>
       <c r="I51" s="31"/>
@@ -3205,16 +3281,16 @@
       <c r="D52" s="20"/>
       <c r="E52" s="35"/>
       <c r="F52" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="G52" s="48" t="s">
-        <v>286</v>
-      </c>
-      <c r="H52" s="49" t="s">
-        <v>287</v>
-      </c>
-      <c r="I52" s="50" t="s">
-        <v>288</v>
+        <v>280</v>
+      </c>
+      <c r="G52" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="H52" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="I52" s="49" t="s">
+        <v>283</v>
       </c>
       <c r="J52" s="31"/>
       <c r="K52" s="31"/>
@@ -3234,10 +3310,10 @@
       <c r="D53" s="20"/>
       <c r="E53" s="35"/>
       <c r="F53" s="17" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H53" s="30"/>
       <c r="I53" s="31"/>
@@ -3253,15 +3329,15 @@
       <c r="B54" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="51" t="s">
-        <v>291</v>
-      </c>
-      <c r="D54" s="51"/>
-      <c r="E54" s="52" t="s">
-        <v>292</v>
+      <c r="C54" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="D54" s="17"/>
+      <c r="E54" s="73" t="s">
+        <v>287</v>
       </c>
       <c r="F54" s="17"/>
-      <c r="G54" s="34"/>
+      <c r="G54" s="36"/>
       <c r="H54" s="30"/>
       <c r="I54" s="31"/>
       <c r="J54" s="31"/>
@@ -3270,21 +3346,21 @@
       <c r="M54" s="33"/>
     </row>
     <row r="55" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="53">
+      <c r="A55" s="51">
         <v>54</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="C55" s="52" t="s">
-        <v>294</v>
-      </c>
-      <c r="D55" s="51"/>
-      <c r="E55" s="52" t="s">
-        <v>295</v>
+        <v>288</v>
+      </c>
+      <c r="C55" s="73" t="s">
+        <v>289</v>
+      </c>
+      <c r="D55" s="17"/>
+      <c r="E55" s="73" t="s">
+        <v>290</v>
       </c>
       <c r="F55" s="17"/>
-      <c r="G55" s="34"/>
+      <c r="G55" s="36"/>
       <c r="H55" s="30"/>
       <c r="I55" s="31"/>
       <c r="J55" s="31"/>
@@ -3304,10 +3380,10 @@
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="35" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G56" s="34"/>
       <c r="H56" s="30"/>
@@ -3322,22 +3398,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>166</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="E57" s="51"/>
+        <v>293</v>
+      </c>
+      <c r="E57" s="50"/>
       <c r="F57" s="17" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>300</v>
-      </c>
-      <c r="H57" s="54"/>
+        <v>295</v>
+      </c>
+      <c r="H57" s="52"/>
       <c r="I57" s="31"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
@@ -3349,19 +3425,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>169</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E58" s="35" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="30"/>
@@ -3374,19 +3450,19 @@
     <row r="59" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="15"/>
-      <c r="C59" s="55" t="s">
+      <c r="C59" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="D59" s="55" t="s">
+      <c r="D59" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="E59" s="56" t="s">
+      <c r="E59" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="F59" s="57" t="s">
+      <c r="F59" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="G59" s="56" t="s">
+      <c r="G59" s="54" t="s">
         <v>47</v>
       </c>
       <c r="H59" s="15"/>
@@ -3400,10 +3476,10 @@
       <c r="A60" s="24"/>
       <c r="B60" s="33"/>
       <c r="C60" s="30"/>
-      <c r="D60" s="58"/>
+      <c r="D60" s="56"/>
       <c r="E60" s="33"/>
-      <c r="F60" s="59" t="s">
-        <v>304</v>
+      <c r="F60" s="57" t="s">
+        <v>299</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
@@ -3419,8 +3495,8 @@
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="59" t="s">
-        <v>305</v>
+      <c r="F61" s="57" t="s">
+        <v>300</v>
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
@@ -3432,15 +3508,15 @@
     </row>
     <row r="62" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
-      <c r="B62" s="60"/>
+      <c r="B62" s="58"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="62" t="s">
-        <v>306</v>
-      </c>
-      <c r="G62" s="63"/>
-      <c r="H62" s="64"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="60" t="s">
+        <v>301</v>
+      </c>
+      <c r="G62" s="61"/>
+      <c r="H62" s="62"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
@@ -3449,17 +3525,17 @@
     </row>
     <row r="63" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="B63" s="60"/>
+        <v>302</v>
+      </c>
+      <c r="B63" s="58"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
-      <c r="E63" s="61"/>
-      <c r="F63" s="62" t="s">
-        <v>308</v>
-      </c>
-      <c r="G63" s="63"/>
-      <c r="H63" s="64"/>
+      <c r="E63" s="59"/>
+      <c r="F63" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="G63" s="61"/>
+      <c r="H63" s="62"/>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
       <c r="K63" s="11"/>
@@ -3472,8 +3548,8 @@
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="59" t="s">
-        <v>309</v>
+      <c r="F64" s="57" t="s">
+        <v>304</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="15"/>

</xml_diff>

<commit_message>
added check mobile messages
</commit_message>
<xml_diff>
--- a/IP echipamente statii.xlsx
+++ b/IP echipamente statii.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83A5EF4-F90D-4DC4-8D62-83BC46ABDEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20D0C97-3C8F-4AFD-BD45-8AF8A1165ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,9 +1000,6 @@
     <t>Catedrala spre policlinica</t>
   </si>
   <si>
-    <t>Autogara TVM nemontat</t>
-  </si>
-  <si>
     <t>192.168.35.58</t>
   </si>
   <si>
@@ -1022,6 +1019,9 @@
   </si>
   <si>
     <t>x192.168.25.45</t>
+  </si>
+  <si>
+    <t>Autogara</t>
   </si>
 </sst>
 </file>
@@ -1967,8 +1967,8 @@
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2482,7 +2482,7 @@
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
       <c r="F19" s="65" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G19" s="36" t="s">
         <v>224</v>
@@ -2883,7 +2883,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>128</v>
@@ -2897,7 +2897,7 @@
         <v>254</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I36" s="31"/>
       <c r="J36" s="31"/>
@@ -3070,7 +3070,7 @@
         <v>309</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="35"/>
@@ -3095,7 +3095,7 @@
         <v>143</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="35"/>
@@ -3150,7 +3150,7 @@
       <c r="D47" s="20"/>
       <c r="E47" s="35"/>
       <c r="F47" s="36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G47" s="34" t="s">
         <v>268</v>
@@ -3196,7 +3196,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>153</v>
@@ -3251,7 +3251,7 @@
         <v>156</v>
       </c>
       <c r="C51" s="74" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="35"/>

</xml_diff>

<commit_message>
commit before start TPL Alerts 2.0 with NodeJS. This is the last stable version of TPL Alerts 1.0
</commit_message>
<xml_diff>
--- a/IP echipamente statii.xlsx
+++ b/IP echipamente statii.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019A82B3-5AF5-4D89-BE93-6F8130FE2B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12073E63-E8DA-433F-9BD0-7E1FDED674B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1967,8 +1967,8 @@
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>